<commit_message>
Update Presets and save feature
</commit_message>
<xml_diff>
--- a/Presets.xlsx
+++ b/Presets.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Type</t>
   </si>
@@ -31,13 +31,34 @@
     <t>Yield_high</t>
   </si>
   <si>
-    <t>Super Efficient Reaction</t>
-  </si>
-  <si>
     <t>Terrible Chromatography</t>
   </si>
   <si>
     <t>Mediocre Telescope</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Efficient Reaction</t>
+  </si>
+  <si>
+    <t>Catalysis</t>
+  </si>
+  <si>
+    <t>Purification</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Great Chromatography</t>
+  </si>
+  <si>
+    <t>OK Reaction</t>
   </si>
 </sst>
 </file>
@@ -392,87 +413,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
+      <c r="E2" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>10000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="C3">
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>120</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
         <v>10000</v>
       </c>
-      <c r="D3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="E7" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>50</v>
-      </c>
-      <c r="C4">
-        <v>120</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.65</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.85</v>
+      <c r="F7" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add additional reaction data
</commit_message>
<xml_diff>
--- a/Presets.xlsx
+++ b/Presets.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albrechj\OneDrive - Bristol-Myers Squibb (O365-D)\2018\PMI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albrechj\OneDrive - Bristol-Myers Squibb (O365-D)\2019\PMI\PMI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7860"/>
   </bookViews>
   <sheets>
-    <sheet name="app_preset_ranges_all_company_c" sheetId="1" r:id="rId1"/>
+    <sheet name="app_preset_ranges_Dec_2018" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="144">
   <si>
     <t>Type</t>
   </si>
@@ -42,410 +42,412 @@
     <t>Addition, 1,2-</t>
   </si>
   <si>
+    <t>Addition, 1,4-</t>
+  </si>
+  <si>
+    <t>Alcohol Dehydration</t>
+  </si>
+  <si>
+    <t>Alcohol Oxidation</t>
+  </si>
+  <si>
+    <t>Aldol/Claisen Addition/Condensation</t>
+  </si>
+  <si>
+    <t>Alkene Reduction</t>
+  </si>
+  <si>
+    <t>Alkene/Alkyne Hydration</t>
+  </si>
+  <si>
+    <t>Alkyne Reduction</t>
+  </si>
+  <si>
+    <t>Alpha Acylation</t>
+  </si>
+  <si>
+    <t>Alpha Alkylation</t>
+  </si>
+  <si>
+    <t>Alpha Arylation</t>
+  </si>
+  <si>
+    <t>Amidation</t>
+  </si>
+  <si>
+    <t>Amide Dehydration to Nitrile</t>
+  </si>
+  <si>
+    <t>Amide Hydrolysis</t>
+  </si>
+  <si>
+    <t>Amidine Formation</t>
+  </si>
+  <si>
+    <t>Arene Reduction</t>
+  </si>
+  <si>
+    <t>Baeyer-Villiger</t>
+  </si>
+  <si>
+    <t>Bioconjugation</t>
+  </si>
+  <si>
+    <t>Bromodehydration</t>
+  </si>
+  <si>
+    <t>C-B coupling</t>
+  </si>
+  <si>
+    <t>C-B Oxidation</t>
+  </si>
+  <si>
+    <t>C-H Oxidation</t>
+  </si>
+  <si>
+    <t>C-N coupling</t>
+  </si>
+  <si>
+    <t>C-O coupling</t>
+  </si>
+  <si>
+    <t>Carbamate Formation</t>
+  </si>
+  <si>
+    <t>Carbonate Formation</t>
+  </si>
+  <si>
+    <t>Carbonyl Oxidation</t>
+  </si>
+  <si>
+    <t>Carbonyl Protection</t>
+  </si>
+  <si>
+    <t>Carbonyl Reduction</t>
+  </si>
+  <si>
+    <t>Carboxylic Acid Activation</t>
+  </si>
+  <si>
+    <t>Chiral Auxiliary Cleavage</t>
+  </si>
+  <si>
+    <t>Chiral Auxiliary Installation</t>
+  </si>
+  <si>
+    <t>Chlorodehydration</t>
+  </si>
+  <si>
+    <t>Chromatography</t>
+  </si>
+  <si>
+    <t>Condensation: Enamine Formation</t>
+  </si>
+  <si>
+    <t>Condensation: Imine Formation</t>
+  </si>
+  <si>
+    <t>Condensation: Oxime/Hydrazone Formation</t>
+  </si>
+  <si>
+    <t>Cope/Claisen Rearrangement</t>
+  </si>
+  <si>
+    <t>Curtius/Hofmann/Lossen/Schmidt Rearrangement</t>
+  </si>
+  <si>
+    <t>Cyanation</t>
+  </si>
+  <si>
+    <t>Cycloaddition</t>
+  </si>
+  <si>
+    <t>Cycloalkylation</t>
+  </si>
+  <si>
+    <t>Cyclocondensation</t>
+  </si>
+  <si>
+    <t>Decarboxylation</t>
+  </si>
+  <si>
+    <t>Dehydrogenation</t>
+  </si>
+  <si>
+    <t>Deoxygenation</t>
+  </si>
+  <si>
+    <t>Deprotection</t>
+  </si>
+  <si>
+    <t>Diazotization</t>
+  </si>
+  <si>
+    <t>Direct Arylation</t>
+  </si>
+  <si>
+    <t>Displacement with CN or N3</t>
+  </si>
+  <si>
+    <t>Electrophilic Aromatic Nitration</t>
+  </si>
+  <si>
+    <t>Enol-Sulfonate/Enol-Phosphate/Enol-Silane Formation</t>
+  </si>
+  <si>
+    <t>Epoxidation</t>
+  </si>
+  <si>
+    <t>Ester Hydrolysis</t>
+  </si>
+  <si>
+    <t>Esterification</t>
+  </si>
+  <si>
+    <t>Fischer Indole Synthesis</t>
+  </si>
+  <si>
+    <t>Fluorodehydration</t>
+  </si>
+  <si>
+    <t>Form Conversion</t>
+  </si>
+  <si>
+    <t>Friedel-Crafts Acylation</t>
+  </si>
+  <si>
+    <t>Friedel-Crafts Alkylation</t>
+  </si>
+  <si>
+    <t>Glycosylation</t>
+  </si>
+  <si>
+    <t>H-X Elimination</t>
+  </si>
+  <si>
+    <t>Halogen/Metal exchange</t>
+  </si>
+  <si>
+    <t>Horner-Wadsworth-Emmons Olefination</t>
+  </si>
+  <si>
+    <t>Iododehydration</t>
+  </si>
+  <si>
+    <t>Isomerization</t>
+  </si>
+  <si>
+    <t>Knöevenagel Condensation</t>
+  </si>
+  <si>
+    <t>Macrolactamization/Macrolactonization</t>
+  </si>
+  <si>
+    <t>Methylation</t>
+  </si>
+  <si>
+    <t>Mitsunobu</t>
+  </si>
+  <si>
+    <t>N-Oxidation</t>
+  </si>
+  <si>
+    <t>N-Protection</t>
+  </si>
+  <si>
+    <t>NAS: Carbon Nucleophile</t>
+  </si>
+  <si>
+    <t>NAS: Nitrogen Nucleophile</t>
+  </si>
+  <si>
+    <t>NAS: Other Nucleophile</t>
+  </si>
+  <si>
+    <t>NAS: Oxygen Nucleophile</t>
+  </si>
+  <si>
+    <t>Negishi/Kumada</t>
+  </si>
+  <si>
+    <t>Nitrile Hydration</t>
+  </si>
+  <si>
+    <t>Nitro Reduction</t>
+  </si>
+  <si>
+    <t>O-Protection</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Other Acyl Substitution</t>
+  </si>
+  <si>
+    <t>Other Alkylation</t>
+  </si>
+  <si>
+    <t>Other Aromatic Substitution</t>
+  </si>
+  <si>
+    <t>Other C-C Transition Metal Coupling</t>
+  </si>
+  <si>
+    <t>Other Carbonyl Chemistry</t>
+  </si>
+  <si>
+    <t>Other Halogenation</t>
+  </si>
+  <si>
+    <t>Other Heteroatom Activation</t>
+  </si>
+  <si>
+    <t>Other Hydration/Dehydration</t>
+  </si>
+  <si>
+    <t>Other Oxidation</t>
+  </si>
+  <si>
+    <t>Other Protection</t>
+  </si>
+  <si>
+    <t>Other Rearrangement</t>
+  </si>
+  <si>
+    <t>Other Reduction</t>
+  </si>
+  <si>
+    <t>Other Ring Formation</t>
+  </si>
+  <si>
+    <t>Oxidative Bromination</t>
+  </si>
+  <si>
+    <t>Oxidative Chlorination</t>
+  </si>
+  <si>
+    <t>Oxidative Cleavage</t>
+  </si>
+  <si>
+    <t>Oxidative Fluorination</t>
+  </si>
+  <si>
+    <t>Oxidative Iodination</t>
+  </si>
+  <si>
+    <t>Phosphinylation/Phosphorylation</t>
+  </si>
+  <si>
+    <t>RCM</t>
+  </si>
+  <si>
+    <t>Recrystallization</t>
+  </si>
+  <si>
+    <t>Reductive Amination</t>
+  </si>
+  <si>
+    <t>Reductive Dehalogenation</t>
+  </si>
+  <si>
+    <t>Resolution: Catalytic</t>
+  </si>
+  <si>
+    <t>Resolution: Classical</t>
+  </si>
+  <si>
+    <t>Ring Contraction</t>
+  </si>
+  <si>
+    <t>Ring Expansion</t>
+  </si>
+  <si>
+    <t>S-Oxidation</t>
+  </si>
+  <si>
+    <t>Salt Break</t>
+  </si>
+  <si>
+    <t>Salt Formation</t>
+  </si>
+  <si>
+    <t>Sandmeyer Reaction</t>
+  </si>
+  <si>
+    <t>Solid-phase Peptide/Oligonucleotide Synthesis</t>
+  </si>
+  <si>
+    <t>Sonogashira</t>
+  </si>
+  <si>
+    <t>Strecker</t>
+  </si>
+  <si>
+    <t>Sulfinylation/Sulfonylation</t>
+  </si>
+  <si>
+    <t>Suzuki</t>
+  </si>
+  <si>
+    <t>Telescope</t>
+  </si>
+  <si>
+    <t>Transesterification</t>
+  </si>
+  <si>
+    <t>Urea Formation</t>
+  </si>
+  <si>
+    <t>Witting Olefination</t>
+  </si>
+  <si>
+    <t>Other Metallation_x000D_</t>
+  </si>
+  <si>
     <t>Carbonyl Chemistry</t>
   </si>
   <si>
-    <t>Addition, 1,4-</t>
-  </si>
-  <si>
-    <t>Alcohol Oxidation</t>
-  </si>
-  <si>
     <t>Oxidation</t>
   </si>
   <si>
-    <t>Aldol/Claisen Addition/Condensation</t>
-  </si>
-  <si>
-    <t>Alkene Reduction</t>
-  </si>
-  <si>
     <t>Reduction</t>
   </si>
   <si>
-    <t>Alkene/Alkyne Hydration</t>
-  </si>
-  <si>
     <t>Hydration/Dehydration</t>
   </si>
   <si>
-    <t>Alkyne Reduction</t>
-  </si>
-  <si>
-    <t>Alpha Acylation</t>
-  </si>
-  <si>
-    <t>Alpha Alkylation</t>
-  </si>
-  <si>
     <t>Alkylation</t>
   </si>
   <si>
-    <t>Alpha Arylation</t>
-  </si>
-  <si>
     <t>C-C Transition Metal Coupling</t>
   </si>
   <si>
-    <t>Amidation</t>
-  </si>
-  <si>
     <t>Acyl Substitution</t>
   </si>
   <si>
-    <t>Amide Dehydration to Nitrile</t>
-  </si>
-  <si>
-    <t>Amide Hydrolysis</t>
-  </si>
-  <si>
-    <t>Amidine Formation</t>
-  </si>
-  <si>
-    <t>Arene Reduction</t>
-  </si>
-  <si>
-    <t>Baeyer-Villiger</t>
-  </si>
-  <si>
-    <t>Bioconjugation</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Bromodehydration</t>
-  </si>
-  <si>
     <t>Halogenation</t>
   </si>
   <si>
-    <t>C-B coupling</t>
-  </si>
-  <si>
     <t>C-X Transition Metal Coupling</t>
   </si>
   <si>
-    <t>C-B Oxidation</t>
-  </si>
-  <si>
-    <t>C-H Oxidation</t>
-  </si>
-  <si>
-    <t>C-N coupling</t>
-  </si>
-  <si>
-    <t>C-O coupling</t>
-  </si>
-  <si>
-    <t>Carbamate Formation</t>
-  </si>
-  <si>
-    <t>Carbonate Formation</t>
-  </si>
-  <si>
-    <t>Carbonyl Protection</t>
-  </si>
-  <si>
     <t>Protection/Deprotection</t>
   </si>
   <si>
-    <t>Carbonyl Reduction</t>
-  </si>
-  <si>
-    <t>Carboxylic Acid Activation</t>
-  </si>
-  <si>
-    <t>Chiral Auxiliary Cleavage</t>
-  </si>
-  <si>
-    <t>Chiral Auxiliary Installation</t>
-  </si>
-  <si>
-    <t>Chlorodehydration</t>
-  </si>
-  <si>
-    <t>Chromatography</t>
-  </si>
-  <si>
-    <t>Condensation: Enamine Formation</t>
-  </si>
-  <si>
-    <t>Condensation: Imine Formation</t>
-  </si>
-  <si>
-    <t>Condensation: Oxime/Hydrazone Formation</t>
-  </si>
-  <si>
-    <t>Cope/Claisen Rearrangement</t>
-  </si>
-  <si>
     <t>Rearrangement</t>
   </si>
   <si>
-    <t>Curtius/Hofmann/Lossen/Schmidt Rearrangement</t>
-  </si>
-  <si>
-    <t>Cyanation</t>
-  </si>
-  <si>
-    <t>Cycloaddition</t>
-  </si>
-  <si>
     <t>Ring Formation</t>
   </si>
   <si>
-    <t>Cycloalkylation</t>
-  </si>
-  <si>
-    <t>Cyclocondensation</t>
-  </si>
-  <si>
-    <t>Decarboxylation</t>
-  </si>
-  <si>
-    <t>Dehydrogenation</t>
-  </si>
-  <si>
-    <t>Deoxygenation</t>
-  </si>
-  <si>
-    <t>Deprotection</t>
-  </si>
-  <si>
-    <t>Diazotization</t>
-  </si>
-  <si>
-    <t>Direct Arylation</t>
-  </si>
-  <si>
-    <t>Displacement with CN or N3</t>
-  </si>
-  <si>
-    <t>Electrophilic Aromatic Nitration</t>
-  </si>
-  <si>
     <t>Aromatic Substitution</t>
   </si>
   <si>
-    <t>Enol-Sulfonate/Enol-Phosphate/Enol-Silane Formation</t>
-  </si>
-  <si>
-    <t>Epoxidation</t>
-  </si>
-  <si>
-    <t>Ester Hydrolysis</t>
-  </si>
-  <si>
-    <t>Esterification</t>
-  </si>
-  <si>
-    <t>Fischer Indole Synthesis</t>
-  </si>
-  <si>
-    <t>Fluorodehydration</t>
-  </si>
-  <si>
-    <t>Form Conversion</t>
-  </si>
-  <si>
-    <t>Friedel-Crafts Acylation</t>
-  </si>
-  <si>
-    <t>Friedel-Crafts Alkylation</t>
-  </si>
-  <si>
-    <t>Glycosylation</t>
-  </si>
-  <si>
-    <t>H-X Elimination</t>
-  </si>
-  <si>
-    <t>Halogen/Metal exchange</t>
-  </si>
-  <si>
     <t>C-M Bond Forming</t>
   </si>
   <si>
-    <t>Horner-Wadsworth-Emmons Olefination</t>
-  </si>
-  <si>
-    <t>Iododehydration</t>
-  </si>
-  <si>
-    <t>Isomerization</t>
-  </si>
-  <si>
-    <t>Knöevenagel Condensation</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Macrolactamization/Macrolactonization</t>
-  </si>
-  <si>
-    <t>Methylation</t>
-  </si>
-  <si>
-    <t>Mitsunobu</t>
-  </si>
-  <si>
     <t>Heteroatom Activation</t>
-  </si>
-  <si>
-    <t>N-Oxidation</t>
-  </si>
-  <si>
-    <t>N-Protection</t>
-  </si>
-  <si>
-    <t>NAS: Carbon Nucleophile</t>
-  </si>
-  <si>
-    <t>NAS: Nitrogen Nucleophile</t>
-  </si>
-  <si>
-    <t>NAS: Other Nucleophile</t>
-  </si>
-  <si>
-    <t>NAS: Oxygen Nucleophile</t>
-  </si>
-  <si>
-    <t>Negishi/Kumada</t>
-  </si>
-  <si>
-    <t>Nitrile Hydration</t>
-  </si>
-  <si>
-    <t>Nitro Reduction</t>
-  </si>
-  <si>
-    <t>O-Protection</t>
-  </si>
-  <si>
-    <t>Other Acyl Substitution</t>
-  </si>
-  <si>
-    <t>Other Alkylation</t>
-  </si>
-  <si>
-    <t>Other Aromatic Substitution</t>
-  </si>
-  <si>
-    <t>Other C-C Transition Metal Coupling</t>
-  </si>
-  <si>
-    <t>Other Carbonyl Chemistry</t>
-  </si>
-  <si>
-    <t>Other Halogenation</t>
-  </si>
-  <si>
-    <t>Other Heteroatom Activation</t>
-  </si>
-  <si>
-    <t>Other Hydration/Dehydration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Metallation_x000D__x000D_
-</t>
-  </si>
-  <si>
-    <t>Other Oxidation</t>
-  </si>
-  <si>
-    <t>Other Protection</t>
-  </si>
-  <si>
-    <t>Other Rearrangement</t>
-  </si>
-  <si>
-    <t>Other Reduction</t>
-  </si>
-  <si>
-    <t>Other Ring Formation</t>
-  </si>
-  <si>
-    <t>Oxidative Bromination</t>
-  </si>
-  <si>
-    <t>Oxidative Chlorination</t>
-  </si>
-  <si>
-    <t>Oxidative Cleavage</t>
-  </si>
-  <si>
-    <t>Oxidative Fluorination</t>
-  </si>
-  <si>
-    <t>Oxidative Iodination</t>
-  </si>
-  <si>
-    <t>Phosphinylation/Phosphorylation</t>
-  </si>
-  <si>
-    <t>RCM</t>
-  </si>
-  <si>
-    <t>Recrystallization</t>
-  </si>
-  <si>
-    <t>Reductive Amination</t>
-  </si>
-  <si>
-    <t>Reductive Dehalogenation</t>
-  </si>
-  <si>
-    <t>Resolution: Catalytic</t>
-  </si>
-  <si>
-    <t>Resolution: Classical</t>
-  </si>
-  <si>
-    <t>Ring Contraction</t>
-  </si>
-  <si>
-    <t>Ring Expansion</t>
-  </si>
-  <si>
-    <t>S-Oxidation</t>
-  </si>
-  <si>
-    <t>Salt Break</t>
-  </si>
-  <si>
-    <t>Salt Formation</t>
-  </si>
-  <si>
-    <t>Sandmeyer Reaction</t>
-  </si>
-  <si>
-    <t>Solid-phase Peptide/Oligonucleotide Synthesis</t>
-  </si>
-  <si>
-    <t>Sonogashira</t>
-  </si>
-  <si>
-    <t>Strecker</t>
-  </si>
-  <si>
-    <t>Sulfinylation/Sulfonylation</t>
-  </si>
-  <si>
-    <t>Suzuki</t>
-  </si>
-  <si>
-    <t>Telescope</t>
-  </si>
-  <si>
-    <t>Transesterification</t>
-  </si>
-  <si>
-    <t>Urea Formation</t>
-  </si>
-  <si>
-    <t>Witting Olefination</t>
   </si>
   <si>
     <t>Category</t>
@@ -1258,10 +1260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G121"/>
+  <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="G116" sqref="G116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,7 +1272,7 @@
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1293,7 +1295,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1301,2572 +1303,2572 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>24</v>
+        <v>24.1</v>
       </c>
       <c r="C2">
-        <v>95.1</v>
+        <v>93.05</v>
       </c>
       <c r="D2">
         <v>0.73</v>
       </c>
       <c r="E2">
-        <v>0.92</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="F2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>14.98</v>
+        <v>13.1</v>
       </c>
       <c r="C3">
-        <v>22.22</v>
+        <v>22.75</v>
       </c>
       <c r="D3">
         <v>0.81</v>
       </c>
       <c r="E3">
-        <v>0.90249999999999997</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="F3">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>22.42</v>
+        <v>51</v>
       </c>
       <c r="C4">
-        <v>40.479999999999997</v>
+        <v>51</v>
       </c>
       <c r="D4">
-        <v>0.83250000000000002</v>
+        <v>0.89</v>
       </c>
       <c r="E4">
-        <v>0.92</v>
+        <v>0.89</v>
       </c>
       <c r="F4">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>9.3000000000000007</v>
+        <v>23.45</v>
       </c>
       <c r="C5">
-        <v>25.6</v>
+        <v>38.35</v>
       </c>
       <c r="D5">
-        <v>0.81</v>
+        <v>0.83</v>
       </c>
       <c r="E5">
-        <v>0.93</v>
+        <v>0.94</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>18.850000000000001</v>
+        <v>10.8</v>
       </c>
       <c r="C6">
-        <v>53.2</v>
+        <v>27.8</v>
       </c>
       <c r="D6">
-        <v>0.81</v>
+        <v>0.76</v>
       </c>
       <c r="E6">
-        <v>0.94</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="F6">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7">
-        <v>28.2</v>
+        <v>18.850000000000001</v>
       </c>
       <c r="C7">
-        <v>28.2</v>
+        <v>53.2</v>
       </c>
       <c r="D7">
-        <v>0.85</v>
+        <v>0.81</v>
       </c>
       <c r="E7">
-        <v>0.85</v>
+        <v>0.94</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>9.9</v>
+        <v>28.2</v>
       </c>
       <c r="C8">
-        <v>35.549999999999997</v>
+        <v>28.2</v>
       </c>
       <c r="D8">
-        <v>0.755</v>
+        <v>0.85</v>
       </c>
       <c r="E8">
-        <v>0.95499999999999996</v>
+        <v>0.85</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>17</v>
+        <v>11.35</v>
       </c>
       <c r="C9">
-        <v>28.5</v>
+        <v>52.825000000000003</v>
       </c>
       <c r="D9">
-        <v>0.73250000000000004</v>
+        <v>0.81499999999999995</v>
       </c>
       <c r="E9">
-        <v>0.94750000000000001</v>
+        <v>0.9375</v>
       </c>
       <c r="F9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>7</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10">
-        <v>11.25</v>
+        <v>17</v>
       </c>
       <c r="C10">
-        <v>68.5</v>
+        <v>28.5</v>
       </c>
       <c r="D10">
-        <v>0.78500000000000003</v>
+        <v>0.73250000000000004</v>
       </c>
       <c r="E10">
-        <v>0.93500000000000005</v>
+        <v>0.94750000000000001</v>
       </c>
       <c r="F10">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>9.6</v>
+      </c>
+      <c r="C11">
+        <v>66.25</v>
+      </c>
+      <c r="D11">
+        <v>0.76749999999999996</v>
+      </c>
+      <c r="E11">
+        <v>0.89749999999999996</v>
+      </c>
+      <c r="F11">
         <v>20</v>
       </c>
-      <c r="B11">
-        <v>22.2</v>
-      </c>
-      <c r="C11">
-        <v>44.35</v>
-      </c>
-      <c r="D11">
-        <v>0.84</v>
-      </c>
-      <c r="E11">
-        <v>0.93</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B12">
-        <v>18.32</v>
+        <v>22.2</v>
       </c>
       <c r="C12">
-        <v>69.55</v>
+        <v>44.35</v>
       </c>
       <c r="D12">
-        <v>0.76500000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="E12">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="F12">
-        <v>108</v>
+        <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B13">
-        <v>11.32</v>
+        <v>19.7</v>
       </c>
       <c r="C13">
-        <v>41.15</v>
+        <v>67.2</v>
       </c>
       <c r="D13">
-        <v>0.78749999999999998</v>
+        <v>0.76749999999999996</v>
       </c>
       <c r="E13">
-        <v>0.90749999999999997</v>
+        <v>0.92</v>
       </c>
       <c r="F13">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B14">
-        <v>30.95</v>
+        <v>12.375</v>
       </c>
       <c r="C14">
-        <v>71.099999999999994</v>
+        <v>30.45</v>
       </c>
       <c r="D14">
-        <v>0.87</v>
+        <v>0.86250000000000004</v>
       </c>
       <c r="E14">
-        <v>0.91500000000000004</v>
+        <v>0.98</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>23</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B15">
-        <v>3.25</v>
+        <v>30.95</v>
       </c>
       <c r="C15">
-        <v>17.75</v>
+        <v>71.099999999999994</v>
       </c>
       <c r="D15">
-        <v>0.72499999999999998</v>
+        <v>0.87</v>
       </c>
       <c r="E15">
-        <v>0.92749999999999999</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="F15">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G15" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B16">
-        <v>12.18</v>
+        <v>3.25</v>
       </c>
       <c r="C16">
-        <v>15.75</v>
+        <v>17.75</v>
       </c>
       <c r="D16">
-        <v>0.87</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="E16">
-        <v>0.95250000000000001</v>
+        <v>0.92749999999999999</v>
       </c>
       <c r="F16">
         <v>6</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B17">
-        <v>105.2</v>
+        <v>12.45</v>
       </c>
       <c r="C17">
-        <v>105.2</v>
+        <v>17.75</v>
       </c>
       <c r="D17">
-        <v>0.8</v>
+        <v>0.88</v>
       </c>
       <c r="E17">
-        <v>0.8</v>
+        <v>0.96</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>10</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B18">
-        <v>2487</v>
+        <v>105.2</v>
       </c>
       <c r="C18">
-        <v>2487</v>
+        <v>105.2</v>
       </c>
       <c r="D18">
-        <v>0.96</v>
+        <v>0.8</v>
       </c>
       <c r="E18">
-        <v>0.96</v>
+        <v>0.8</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>30</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B19">
-        <v>14.05</v>
+        <v>2487.4</v>
       </c>
       <c r="C19">
-        <v>20.65</v>
+        <v>2487.4</v>
       </c>
       <c r="D19">
-        <v>0.88500000000000001</v>
+        <v>0.96</v>
       </c>
       <c r="E19">
-        <v>0.89500000000000002</v>
+        <v>0.96</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B20">
-        <v>12.12</v>
+        <v>14.05</v>
       </c>
       <c r="C20">
-        <v>48.82</v>
+        <v>20.65</v>
       </c>
       <c r="D20">
-        <v>0.78749999999999998</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="E20">
-        <v>0.94750000000000001</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="F20">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B21">
-        <v>51.92</v>
+        <v>12.2</v>
       </c>
       <c r="C21">
-        <v>59.58</v>
+        <v>54.6</v>
       </c>
       <c r="D21">
-        <v>0.88</v>
+        <v>0.8</v>
       </c>
       <c r="E21">
-        <v>0.92</v>
+        <v>0.94</v>
       </c>
       <c r="F21">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B22">
-        <v>23.2</v>
+        <v>51.924999999999997</v>
       </c>
       <c r="C22">
-        <v>23.2</v>
+        <v>59.575000000000003</v>
       </c>
       <c r="D22">
-        <v>0.82</v>
+        <v>0.88</v>
       </c>
       <c r="E22">
-        <v>0.82</v>
+        <v>0.92</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B23">
-        <v>30.25</v>
+        <v>23.2</v>
       </c>
       <c r="C23">
-        <v>125.8</v>
+        <v>23.2</v>
       </c>
       <c r="D23">
-        <v>0.63500000000000001</v>
+        <v>0.82</v>
       </c>
       <c r="E23">
-        <v>0.85</v>
+        <v>0.82</v>
       </c>
       <c r="F23">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>34</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B24">
-        <v>33.1</v>
+        <v>32.125</v>
       </c>
       <c r="C24">
-        <v>80.180000000000007</v>
+        <v>141</v>
       </c>
       <c r="D24">
-        <v>0.66</v>
+        <v>0.63749999999999996</v>
       </c>
       <c r="E24">
-        <v>0.755</v>
+        <v>0.85</v>
       </c>
       <c r="F24">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="G24" t="s">
-        <v>34</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B25">
-        <v>7.1</v>
+        <v>33.1</v>
       </c>
       <c r="C25">
-        <v>28.3</v>
+        <v>80.174999999999997</v>
       </c>
       <c r="D25">
-        <v>0.81</v>
+        <v>0.66</v>
       </c>
       <c r="E25">
-        <v>0.94499999999999995</v>
+        <v>0.755</v>
       </c>
       <c r="F25">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G25" t="s">
-        <v>23</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B26">
-        <v>17.399999999999999</v>
+        <v>8</v>
       </c>
       <c r="C26">
-        <v>17.399999999999999</v>
+        <v>27.35</v>
       </c>
       <c r="D26">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="E26">
-        <v>0.95</v>
+        <v>0.92749999999999999</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B27">
-        <v>34.85</v>
+        <v>16.350000000000001</v>
       </c>
       <c r="C27">
-        <v>36.950000000000003</v>
+        <v>17.05</v>
       </c>
       <c r="D27">
-        <v>0.91249999999999998</v>
+        <v>0.95</v>
       </c>
       <c r="E27">
-        <v>0.9375</v>
+        <v>0.95</v>
       </c>
       <c r="F27">
         <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B28">
-        <v>16.25</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="C28">
-        <v>62.9</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="D28">
-        <v>0.81499999999999995</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>0.97499999999999998</v>
+        <v>1</v>
       </c>
       <c r="F28">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B29">
-        <v>3.6749999999999998</v>
+        <v>20</v>
       </c>
       <c r="C29">
-        <v>12.52</v>
+        <v>34.85</v>
       </c>
       <c r="D29">
-        <v>0.875</v>
+        <v>0.92</v>
       </c>
       <c r="E29">
-        <v>0.94</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="F29">
         <v>4</v>
       </c>
       <c r="G29" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B30">
-        <v>37.92</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="C30">
-        <v>126.3</v>
+        <v>95.45</v>
       </c>
       <c r="D30">
-        <v>0.84499999999999997</v>
+        <v>0.8125</v>
       </c>
       <c r="E30">
-        <v>0.9375</v>
+        <v>0.96250000000000002</v>
       </c>
       <c r="F30">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="G30" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B31">
-        <v>27.3</v>
+        <v>3.6749999999999998</v>
       </c>
       <c r="C31">
-        <v>66.099999999999994</v>
+        <v>12.525</v>
       </c>
       <c r="D31">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="E31">
-        <v>0.91500000000000004</v>
+        <v>0.94</v>
       </c>
       <c r="F31">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G31" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B32">
-        <v>19.5</v>
+        <v>37.924999999999997</v>
       </c>
       <c r="C32">
-        <v>44.95</v>
+        <v>126.325</v>
       </c>
       <c r="D32">
-        <v>0.82</v>
+        <v>0.84499999999999997</v>
       </c>
       <c r="E32">
-        <v>0.92500000000000004</v>
+        <v>0.9375</v>
       </c>
       <c r="F32">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G32" t="s">
-        <v>32</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B33">
-        <v>715</v>
+        <v>27.3</v>
       </c>
       <c r="C33">
-        <v>8574</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="D33">
-        <v>0.41</v>
+        <v>0.625</v>
       </c>
       <c r="E33">
-        <v>0.86499999999999999</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="F33">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G33" t="s">
-        <v>30</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B34">
-        <v>7.8250000000000002</v>
+        <v>18.05</v>
       </c>
       <c r="C34">
-        <v>16.149999999999999</v>
+        <v>44.424999999999997</v>
       </c>
       <c r="D34">
-        <v>0.76</v>
+        <v>0.82</v>
       </c>
       <c r="E34">
-        <v>0.96750000000000003</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="F34">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G34" t="s">
-        <v>7</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B35">
-        <v>10.6</v>
+        <v>714.95</v>
       </c>
       <c r="C35">
-        <v>24.1</v>
+        <v>8573.8250000000007</v>
       </c>
       <c r="D35">
-        <v>0.9</v>
+        <v>0.41</v>
       </c>
       <c r="E35">
-        <v>0.94</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="F35">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G35" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B36">
-        <v>11.18</v>
+        <v>7.8250000000000002</v>
       </c>
       <c r="C36">
-        <v>27.5</v>
+        <v>16.149999999999999</v>
       </c>
       <c r="D36">
-        <v>0.78500000000000003</v>
+        <v>0.76</v>
       </c>
       <c r="E36">
-        <v>0.89249999999999996</v>
+        <v>0.96750000000000003</v>
       </c>
       <c r="F36">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G36" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B37">
-        <v>27.7</v>
+        <v>10.6</v>
       </c>
       <c r="C37">
-        <v>27.7</v>
+        <v>24.1</v>
       </c>
       <c r="D37">
-        <v>0.92</v>
+        <v>0.9</v>
       </c>
       <c r="E37">
-        <v>0.92</v>
+        <v>0.94</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G37" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B38">
-        <v>32.72</v>
+        <v>12.2</v>
       </c>
       <c r="C38">
-        <v>69.05</v>
+        <v>29</v>
       </c>
       <c r="D38">
-        <v>0.77749999999999997</v>
+        <v>0.8</v>
       </c>
       <c r="E38">
-        <v>0.88249999999999995</v>
+        <v>0.9</v>
       </c>
       <c r="F38">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B39">
-        <v>69.599999999999994</v>
+        <v>27.7</v>
       </c>
       <c r="C39">
-        <v>101</v>
+        <v>27.7</v>
       </c>
       <c r="D39">
-        <v>0.72</v>
+        <v>0.92</v>
       </c>
       <c r="E39">
-        <v>0.89</v>
+        <v>0.92</v>
       </c>
       <c r="F39">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>21</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B40">
-        <v>20.8</v>
+        <v>36.549999999999997</v>
       </c>
       <c r="C40">
-        <v>53.62</v>
+        <v>64.924999999999997</v>
       </c>
       <c r="D40">
-        <v>0.74750000000000005</v>
+        <v>0.73250000000000004</v>
       </c>
       <c r="E40">
-        <v>0.9425</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="F40">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G40" t="s">
-        <v>57</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B41">
-        <v>26.65</v>
+        <v>69.599999999999994</v>
       </c>
       <c r="C41">
-        <v>58.5</v>
+        <v>101</v>
       </c>
       <c r="D41">
-        <v>0.72499999999999998</v>
+        <v>0.72</v>
       </c>
       <c r="E41">
-        <v>0.90500000000000003</v>
+        <v>0.89</v>
       </c>
       <c r="F41">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G41" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B42">
-        <v>25.15</v>
+        <v>21.2</v>
       </c>
       <c r="C42">
-        <v>60.8</v>
+        <v>52.6</v>
       </c>
       <c r="D42">
-        <v>0.63</v>
+        <v>0.71</v>
       </c>
       <c r="E42">
-        <v>0.89</v>
+        <v>0.93</v>
       </c>
       <c r="F42">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="G42" t="s">
-        <v>7</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B43">
-        <v>21.7</v>
+        <v>26.65</v>
       </c>
       <c r="C43">
-        <v>27.1</v>
+        <v>58.5</v>
       </c>
       <c r="D43">
-        <v>0.86499999999999999</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="E43">
-        <v>0.94499999999999995</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="F43">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G43" t="s">
-        <v>53</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B44">
-        <v>50.62</v>
+        <v>26.25</v>
       </c>
       <c r="C44">
-        <v>53.97</v>
+        <v>63.475000000000001</v>
       </c>
       <c r="D44">
-        <v>0.84250000000000003</v>
+        <v>0.62250000000000005</v>
       </c>
       <c r="E44">
-        <v>0.9</v>
+        <v>0.88749999999999996</v>
       </c>
       <c r="F44">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="G44" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B45">
-        <v>26</v>
+        <v>24.4</v>
       </c>
       <c r="C45">
-        <v>124.9</v>
+        <v>28.824999999999999</v>
       </c>
       <c r="D45">
-        <v>0.86250000000000004</v>
+        <v>0.78749999999999998</v>
       </c>
       <c r="E45">
-        <v>0.95499999999999996</v>
+        <v>0.9425</v>
       </c>
       <c r="F45">
         <v>4</v>
       </c>
       <c r="G45" t="s">
-        <v>13</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B46">
-        <v>19.2</v>
+        <v>50.625</v>
       </c>
       <c r="C46">
-        <v>69.5</v>
+        <v>53.975000000000001</v>
       </c>
       <c r="D46">
-        <v>0.85</v>
+        <v>0.84250000000000003</v>
       </c>
       <c r="E46">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="F46">
-        <v>81</v>
+        <v>6</v>
       </c>
       <c r="G46" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B47">
-        <v>37.020000000000003</v>
+        <v>26</v>
       </c>
       <c r="C47">
-        <v>55.28</v>
+        <v>124.925</v>
       </c>
       <c r="D47">
-        <v>0.75749999999999995</v>
+        <v>0.86250000000000004</v>
       </c>
       <c r="E47">
-        <v>0.77249999999999996</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="F47">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G47" t="s">
-        <v>10</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B48">
-        <v>67.849999999999994</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="C48">
-        <v>96.45</v>
+        <v>72.125</v>
       </c>
       <c r="D48">
-        <v>0.62</v>
+        <v>0.84250000000000003</v>
       </c>
       <c r="E48">
-        <v>0.745</v>
+        <v>0.95</v>
       </c>
       <c r="F48">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="G48" t="s">
-        <v>21</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B49">
-        <v>14.7</v>
+        <v>37.024999999999999</v>
       </c>
       <c r="C49">
-        <v>73.27</v>
+        <v>55.274999999999999</v>
       </c>
       <c r="D49">
-        <v>0.64749999999999996</v>
+        <v>0.75749999999999995</v>
       </c>
       <c r="E49">
-        <v>0.94750000000000001</v>
+        <v>0.77249999999999996</v>
       </c>
       <c r="F49">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G49" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B50">
-        <v>39.619999999999997</v>
+        <v>67.849999999999994</v>
       </c>
       <c r="C50">
-        <v>66.680000000000007</v>
+        <v>96.45</v>
       </c>
       <c r="D50">
-        <v>0.77500000000000002</v>
+        <v>0.62</v>
       </c>
       <c r="E50">
-        <v>0.91</v>
+        <v>0.745</v>
       </c>
       <c r="F50">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G50" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B51">
-        <v>8</v>
+        <v>17.5</v>
       </c>
       <c r="C51">
-        <v>8</v>
+        <v>58.3</v>
       </c>
       <c r="D51">
-        <v>0.7</v>
+        <v>0.64749999999999996</v>
       </c>
       <c r="E51">
-        <v>0.7</v>
+        <v>0.94750000000000001</v>
       </c>
       <c r="F51">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G51" t="s">
-        <v>7</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B52">
-        <v>20.05</v>
+        <v>40.024999999999999</v>
       </c>
       <c r="C52">
-        <v>40.25</v>
+        <v>67.224999999999994</v>
       </c>
       <c r="D52">
-        <v>0.91500000000000004</v>
+        <v>0.8</v>
       </c>
       <c r="E52">
-        <v>0.98</v>
+        <v>0.91</v>
       </c>
       <c r="F52">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="G52" t="s">
-        <v>10</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B53">
-        <v>14.2</v>
+        <v>8</v>
       </c>
       <c r="C53">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="D53">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="E53">
-        <v>0.96</v>
+        <v>0.7</v>
       </c>
       <c r="F53">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B54">
-        <v>12.4</v>
+        <v>20.05</v>
       </c>
       <c r="C54">
-        <v>37.5</v>
+        <v>40.25</v>
       </c>
       <c r="D54">
-        <v>0.86</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="E54">
-        <v>0.96</v>
+        <v>0.98</v>
       </c>
       <c r="F54">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="G54" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B55">
-        <v>58.3</v>
+        <v>15.2</v>
       </c>
       <c r="C55">
-        <v>70.319999999999993</v>
+        <v>68.375</v>
       </c>
       <c r="D55">
-        <v>0.55249999999999999</v>
+        <v>0.79</v>
       </c>
       <c r="E55">
-        <v>0.67749999999999999</v>
+        <v>0.96</v>
       </c>
       <c r="F55">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="G55" t="s">
-        <v>53</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B56">
-        <v>33.97</v>
+        <v>12.4</v>
       </c>
       <c r="C56">
-        <v>75.88</v>
+        <v>42</v>
       </c>
       <c r="D56">
-        <v>0.60250000000000004</v>
+        <v>0.85750000000000004</v>
       </c>
       <c r="E56">
-        <v>0.78249999999999997</v>
+        <v>0.96</v>
       </c>
       <c r="F56">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="G56" t="s">
-        <v>32</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B57">
-        <v>21.08</v>
+        <v>58.3</v>
       </c>
       <c r="C57">
-        <v>43.75</v>
+        <v>70.325000000000003</v>
       </c>
       <c r="D57">
-        <v>0.89249999999999996</v>
+        <v>0.55249999999999999</v>
       </c>
       <c r="E57">
-        <v>0.93</v>
+        <v>0.67749999999999999</v>
       </c>
       <c r="F57">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G57" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B58">
-        <v>20.9</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="C58">
-        <v>72.599999999999994</v>
+        <v>90</v>
       </c>
       <c r="D58">
-        <v>0.73</v>
+        <v>0.62</v>
       </c>
       <c r="E58">
-        <v>0.89</v>
+        <v>0.79</v>
       </c>
       <c r="F58">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G58" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B59">
-        <v>12.9</v>
+        <v>21.074999999999999</v>
       </c>
       <c r="C59">
-        <v>31</v>
+        <v>43.75</v>
       </c>
       <c r="D59">
-        <v>0.84</v>
+        <v>0.89249999999999996</v>
       </c>
       <c r="E59">
-        <v>0.85</v>
+        <v>0.93</v>
       </c>
       <c r="F59">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G59" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B60">
-        <v>12.08</v>
+        <v>20.5</v>
       </c>
       <c r="C60">
-        <v>65.849999999999994</v>
+        <v>70.95</v>
       </c>
       <c r="D60">
-        <v>0.59499999999999997</v>
+        <v>0.73750000000000004</v>
       </c>
       <c r="E60">
-        <v>0.6925</v>
+        <v>0.89749999999999996</v>
       </c>
       <c r="F60">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G60" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B61">
-        <v>24.2</v>
+        <v>15.05</v>
       </c>
       <c r="C61">
-        <v>30.6</v>
+        <v>36.024999999999999</v>
       </c>
       <c r="D61">
-        <v>0.85750000000000004</v>
+        <v>0.81</v>
       </c>
       <c r="E61">
-        <v>0.89249999999999996</v>
+        <v>0.85</v>
       </c>
       <c r="F61">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G61" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B62">
-        <v>28.7</v>
+        <v>12.074999999999999</v>
       </c>
       <c r="C62">
-        <v>40.049999999999997</v>
+        <v>65.849999999999994</v>
       </c>
       <c r="D62">
-        <v>0.89500000000000002</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="E62">
-        <v>0.95499999999999996</v>
+        <v>0.6925</v>
       </c>
       <c r="F62">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G62" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B63">
-        <v>23.4</v>
+        <v>24.2</v>
       </c>
       <c r="C63">
-        <v>29.65</v>
+        <v>30.6</v>
       </c>
       <c r="D63">
-        <v>0.77500000000000002</v>
+        <v>0.85750000000000004</v>
       </c>
       <c r="E63">
-        <v>0.86</v>
+        <v>0.89249999999999996</v>
       </c>
       <c r="F63">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G63" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B64">
-        <v>35.299999999999997</v>
+        <v>28.7</v>
       </c>
       <c r="C64">
-        <v>35.299999999999997</v>
+        <v>40.049999999999997</v>
       </c>
       <c r="D64">
-        <v>0.91</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="E64">
-        <v>0.91</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="F64">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G64" t="s">
-        <v>32</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B65">
-        <v>19</v>
+        <v>23.4</v>
       </c>
       <c r="C65">
-        <v>24.8</v>
+        <v>29.65</v>
       </c>
       <c r="D65">
-        <v>0.88</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="E65">
-        <v>0.9</v>
+        <v>0.86</v>
       </c>
       <c r="F65">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G65" t="s">
-        <v>30</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B66">
-        <v>7.4249999999999998</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="C66">
-        <v>19.5</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="D66">
         <v>0.91</v>
       </c>
       <c r="E66">
-        <v>0.97</v>
+        <v>0.91</v>
       </c>
       <c r="F66">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G66" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B67">
-        <v>35.4</v>
+        <v>19</v>
       </c>
       <c r="C67">
-        <v>52.2</v>
+        <v>24.8</v>
       </c>
       <c r="D67">
-        <v>0.96250000000000002</v>
+        <v>0.88</v>
       </c>
       <c r="E67">
-        <v>0.98750000000000004</v>
+        <v>0.9</v>
       </c>
       <c r="F67">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G67" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B68">
-        <v>19.399999999999999</v>
+        <v>7.4249999999999998</v>
       </c>
       <c r="C68">
-        <v>47</v>
+        <v>19.5</v>
       </c>
       <c r="D68">
-        <v>0.78</v>
+        <v>0.91</v>
       </c>
       <c r="E68">
-        <v>0.93</v>
+        <v>0.97</v>
       </c>
       <c r="F68">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="G68" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B69">
-        <v>35.9</v>
+        <v>35.4</v>
       </c>
       <c r="C69">
-        <v>198.7</v>
+        <v>52.2</v>
       </c>
       <c r="D69">
-        <v>0.64</v>
+        <v>0.96250000000000002</v>
       </c>
       <c r="E69">
-        <v>0.82</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="F69">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G69" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B70">
-        <v>35.65</v>
+        <v>20.475000000000001</v>
       </c>
       <c r="C70">
-        <v>52.38</v>
+        <v>57.8</v>
       </c>
       <c r="D70">
-        <v>0.82250000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="E70">
-        <v>0.92500000000000004</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="F70">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="G70" t="s">
-        <v>10</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B71">
-        <v>9.4</v>
+        <v>35.9</v>
       </c>
       <c r="C71">
-        <v>36.6</v>
+        <v>198.7</v>
       </c>
       <c r="D71">
-        <v>0.79500000000000004</v>
+        <v>0.64</v>
       </c>
       <c r="E71">
-        <v>0.91</v>
+        <v>0.82</v>
       </c>
       <c r="F71">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G71" t="s">
-        <v>42</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B72">
-        <v>22</v>
+        <v>35.65</v>
       </c>
       <c r="C72">
-        <v>36.6</v>
+        <v>52.375</v>
       </c>
       <c r="D72">
-        <v>0.78</v>
+        <v>0.82250000000000001</v>
       </c>
       <c r="E72">
-        <v>0.9</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="F72">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G72" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B73">
-        <v>12.8</v>
+        <v>11</v>
       </c>
       <c r="C73">
-        <v>51.8</v>
+        <v>35.174999999999997</v>
       </c>
       <c r="D73">
-        <v>0.8</v>
+        <v>0.83</v>
       </c>
       <c r="E73">
-        <v>0.91</v>
+        <v>0.95</v>
       </c>
       <c r="F73">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="G73" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="B74">
-        <v>20.149999999999999</v>
+        <v>23.5</v>
       </c>
       <c r="C74">
-        <v>26.25</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="D74">
-        <v>0.875</v>
+        <v>0.78</v>
       </c>
       <c r="E74">
-        <v>0.92500000000000004</v>
+        <v>0.9</v>
       </c>
       <c r="F74">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G74" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="B75">
-        <v>17.899999999999999</v>
+        <v>13.3</v>
       </c>
       <c r="C75">
-        <v>53.2</v>
+        <v>51.8</v>
       </c>
       <c r="D75">
-        <v>0.77</v>
+        <v>0.79</v>
       </c>
       <c r="E75">
-        <v>0.95</v>
+        <v>0.92</v>
       </c>
       <c r="F75">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="G75" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="B76">
-        <v>32.6</v>
+        <v>20.149999999999999</v>
       </c>
       <c r="C76">
-        <v>43.62</v>
+        <v>26.25</v>
       </c>
       <c r="D76">
-        <v>0.62749999999999995</v>
+        <v>0.875</v>
       </c>
       <c r="E76">
-        <v>0.86499999999999999</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="F76">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G76" t="s">
-        <v>21</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B77">
-        <v>29.22</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="C77">
-        <v>70.349999999999994</v>
+        <v>53.2</v>
       </c>
       <c r="D77">
-        <v>0.79249999999999998</v>
+        <v>0.77</v>
       </c>
       <c r="E77">
         <v>0.95</v>
       </c>
       <c r="F77">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="G77" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B78">
-        <v>27.1</v>
+        <v>32.6</v>
       </c>
       <c r="C78">
-        <v>66</v>
+        <v>43.625</v>
       </c>
       <c r="D78">
-        <v>0.77</v>
+        <v>0.62749999999999995</v>
       </c>
       <c r="E78">
-        <v>0.93</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="F78">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="G78" t="s">
-        <v>13</v>
+        <v>133</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B79">
-        <v>8.4</v>
+        <v>29.225000000000001</v>
       </c>
       <c r="C79">
-        <v>24.08</v>
+        <v>70.349999999999994</v>
       </c>
       <c r="D79">
-        <v>0.88500000000000001</v>
+        <v>0.79249999999999998</v>
       </c>
       <c r="E79">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="F79">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G79" t="s">
-        <v>42</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="B80">
-        <v>19.600000000000001</v>
+        <v>27.1</v>
       </c>
       <c r="C80">
-        <v>58.2</v>
+        <v>65.474999999999994</v>
       </c>
       <c r="D80">
-        <v>0.74</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="E80">
-        <v>0.93</v>
+        <v>0.92</v>
       </c>
       <c r="F80">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="G80" t="s">
-        <v>30</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B81">
-        <v>12.45</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C81">
-        <v>34.1</v>
+        <v>24.15</v>
       </c>
       <c r="D81">
-        <v>0.85499999999999998</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="E81">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="F81">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G81" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="B82">
-        <v>15.5</v>
+        <v>26</v>
       </c>
       <c r="C82">
-        <v>45.7</v>
+        <v>54</v>
       </c>
       <c r="D82">
-        <v>0.70499999999999996</v>
+        <v>0.82</v>
       </c>
       <c r="E82">
-        <v>0.92500000000000004</v>
+        <v>0.93</v>
       </c>
       <c r="F82">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="G82" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="B83">
-        <v>20.8</v>
+        <v>10.55</v>
       </c>
       <c r="C83">
-        <v>59.5</v>
+        <v>35.1</v>
       </c>
       <c r="D83">
-        <v>0.68</v>
+        <v>0.84499999999999997</v>
       </c>
       <c r="E83">
-        <v>0.92</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="F83">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G83" t="s">
-        <v>68</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B84">
-        <v>20</v>
+        <v>15.6</v>
       </c>
       <c r="C84">
-        <v>59.1</v>
+        <v>46.2</v>
       </c>
       <c r="D84">
-        <v>0.64</v>
+        <v>0.71</v>
       </c>
       <c r="E84">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="F84">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="G84" t="s">
-        <v>21</v>
+        <v>132</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B85">
-        <v>7.8</v>
+        <v>20.8</v>
       </c>
       <c r="C85">
-        <v>30.9</v>
+        <v>59.5</v>
       </c>
       <c r="D85">
-        <v>0.81</v>
+        <v>0.68</v>
       </c>
       <c r="E85">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
       <c r="F85">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G85" t="s">
-        <v>7</v>
+        <v>140</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B86">
-        <v>16.399999999999999</v>
+        <v>20</v>
       </c>
       <c r="C86">
-        <v>16.399999999999999</v>
+        <v>59.1</v>
       </c>
       <c r="D86">
-        <v>0.9</v>
+        <v>0.64</v>
       </c>
       <c r="E86">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="F86">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="G86" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B87">
-        <v>26</v>
+        <v>7.8</v>
       </c>
       <c r="C87">
-        <v>49.8</v>
+        <v>30.9</v>
       </c>
       <c r="D87">
-        <v>0.96750000000000003</v>
+        <v>0.81</v>
       </c>
       <c r="E87">
-        <v>0.98250000000000004</v>
+        <v>0.9</v>
       </c>
       <c r="F87">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G87" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="B88">
-        <v>76.400000000000006</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="C88">
-        <v>382.6</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="D88">
-        <v>0.56499999999999995</v>
+        <v>0.9</v>
       </c>
       <c r="E88">
-        <v>0.85499999999999998</v>
+        <v>0.9</v>
       </c>
       <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89">
+        <v>37.9</v>
+      </c>
+      <c r="C89">
+        <v>66.349999999999994</v>
+      </c>
+      <c r="D89">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="E89">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="F89">
         <v>3</v>
       </c>
-      <c r="G88" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B89">
-        <v>6.375</v>
-      </c>
-      <c r="C89">
-        <v>8.3249999999999993</v>
-      </c>
-      <c r="D89">
-        <v>0.99250000000000005</v>
-      </c>
-      <c r="E89">
-        <v>0.99750000000000005</v>
-      </c>
-      <c r="F89">
-        <v>2</v>
-      </c>
       <c r="G89" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B90">
-        <v>45.5</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="C90">
-        <v>90.5</v>
+        <v>382.65</v>
       </c>
       <c r="D90">
-        <v>0.78249999999999997</v>
+        <v>0.56499999999999995</v>
       </c>
       <c r="E90">
-        <v>0.86750000000000005</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="F90">
+        <v>3</v>
+      </c>
+      <c r="G90" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B91">
+        <v>6.375</v>
+      </c>
+      <c r="C91">
+        <v>8.3249999999999993</v>
+      </c>
+      <c r="D91">
+        <v>0.99250000000000005</v>
+      </c>
+      <c r="E91">
+        <v>0.99750000000000005</v>
+      </c>
+      <c r="F91">
         <v>2</v>
       </c>
-      <c r="G90" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>111</v>
-      </c>
-      <c r="B91">
-        <v>7.7</v>
-      </c>
-      <c r="C91">
-        <v>7.7</v>
-      </c>
-      <c r="D91">
-        <v>0.98</v>
-      </c>
-      <c r="E91">
-        <v>0.98</v>
-      </c>
-      <c r="F91">
-        <v>1</v>
-      </c>
       <c r="G91" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="B92">
-        <v>17.7</v>
+        <v>45.5</v>
       </c>
       <c r="C92">
-        <v>40</v>
+        <v>90.5</v>
       </c>
       <c r="D92">
-        <v>0.76</v>
+        <v>0.78249999999999997</v>
       </c>
       <c r="E92">
-        <v>0.86</v>
+        <v>0.86750000000000005</v>
       </c>
       <c r="F92">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G92" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="B93">
-        <v>29.6</v>
+        <v>7.7</v>
       </c>
       <c r="C93">
-        <v>60.82</v>
+        <v>7.7</v>
       </c>
       <c r="D93">
-        <v>0.70250000000000001</v>
+        <v>0.98</v>
       </c>
       <c r="E93">
-        <v>0.87749999999999995</v>
+        <v>0.98</v>
       </c>
       <c r="F93">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G93" t="s">
-        <v>13</v>
+        <v>137</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="B94">
-        <v>16.45</v>
+        <v>17.824999999999999</v>
       </c>
       <c r="C94">
-        <v>49.9</v>
+        <v>37.25</v>
       </c>
       <c r="D94">
-        <v>0.67500000000000004</v>
+        <v>0.76249999999999996</v>
       </c>
       <c r="E94">
-        <v>0.86</v>
+        <v>0.875</v>
       </c>
       <c r="F94">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="G94" t="s">
-        <v>57</v>
+        <v>138</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="B95">
-        <v>16.2</v>
+        <v>29.8</v>
       </c>
       <c r="C95">
-        <v>50.7</v>
+        <v>61.4</v>
       </c>
       <c r="D95">
-        <v>0.7</v>
+        <v>0.69750000000000001</v>
       </c>
       <c r="E95">
-        <v>0.91</v>
+        <v>0.88</v>
       </c>
       <c r="F95">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="G95" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="B96">
-        <v>15.6</v>
+        <v>16.8</v>
       </c>
       <c r="C96">
-        <v>84.7</v>
+        <v>49.8</v>
       </c>
       <c r="D96">
-        <v>0.75749999999999995</v>
+        <v>0.67</v>
       </c>
       <c r="E96">
-        <v>0.90749999999999997</v>
+        <v>0.86</v>
       </c>
       <c r="F96">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="G96" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B97">
-        <v>67.98</v>
+        <v>16.25</v>
       </c>
       <c r="C97">
-        <v>104.5</v>
+        <v>49.9</v>
       </c>
       <c r="D97">
-        <v>0.59499999999999997</v>
+        <v>0.75249999999999995</v>
       </c>
       <c r="E97">
-        <v>0.64500000000000002</v>
+        <v>0.91749999999999998</v>
       </c>
       <c r="F97">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="G97" t="s">
-        <v>10</v>
+        <v>135</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B98">
-        <v>42.9</v>
+        <v>15.8</v>
       </c>
       <c r="C98">
-        <v>93.35</v>
+        <v>93.3</v>
       </c>
       <c r="D98">
-        <v>0.54500000000000004</v>
+        <v>0.74</v>
       </c>
       <c r="E98">
-        <v>0.86499999999999999</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="F98">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G98" t="s">
-        <v>32</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B99">
-        <v>18.399999999999999</v>
+        <v>67.974999999999994</v>
       </c>
       <c r="C99">
-        <v>32</v>
+        <v>104.52500000000001</v>
       </c>
       <c r="D99">
-        <v>0.84</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="E99">
-        <v>0.95</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="F99">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="G99" t="s">
-        <v>32</v>
+        <v>129</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B100">
-        <v>27.88</v>
+        <v>42.9</v>
       </c>
       <c r="C100">
-        <v>50.03</v>
+        <v>93.35</v>
       </c>
       <c r="D100">
-        <v>0.82499999999999996</v>
+        <v>0.54500000000000004</v>
       </c>
       <c r="E100">
-        <v>0.85499999999999998</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="F100">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G100" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="B101">
-        <v>392.1</v>
+        <v>17.2</v>
       </c>
       <c r="C101">
-        <v>809.6</v>
+        <v>31.7</v>
       </c>
       <c r="D101">
-        <v>0.80500000000000005</v>
+        <v>0.83</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="F101">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="G101" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="B102">
-        <v>15.18</v>
+        <v>27.875</v>
       </c>
       <c r="C102">
-        <v>34.1</v>
+        <v>50.024999999999999</v>
       </c>
       <c r="D102">
-        <v>0.8</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="E102">
-        <v>0.93500000000000005</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="F102">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="G102" t="s">
-        <v>30</v>
+        <v>142</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="B103">
-        <v>20.420000000000002</v>
+        <v>392.07499999999999</v>
       </c>
       <c r="C103">
-        <v>91.15</v>
+        <v>809.65</v>
       </c>
       <c r="D103">
-        <v>0.71750000000000003</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="E103">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="F103">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="G103" t="s">
-        <v>13</v>
+        <v>133</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="B104">
-        <v>56.4</v>
+        <v>15.2</v>
       </c>
       <c r="C104">
-        <v>56.4</v>
+        <v>33.9</v>
       </c>
       <c r="D104">
-        <v>0.67</v>
+        <v>0.8</v>
       </c>
       <c r="E104">
-        <v>0.67</v>
+        <v>0.95</v>
       </c>
       <c r="F104">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="G104" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="B105">
-        <v>39.72</v>
+        <v>22.8</v>
       </c>
       <c r="C105">
-        <v>121.2</v>
+        <v>91.2</v>
       </c>
       <c r="D105">
-        <v>0.36499999999999999</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="E105">
-        <v>0.45500000000000002</v>
+        <v>0.85</v>
       </c>
       <c r="F105">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="G105" t="s">
-        <v>30</v>
+        <v>130</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="B106">
-        <v>35.880000000000003</v>
+        <v>59.55</v>
       </c>
       <c r="C106">
-        <v>90.35</v>
+        <v>65.849999999999994</v>
       </c>
       <c r="D106">
-        <v>0.3175</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="E106">
-        <v>0.42249999999999999</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="F106">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="G106" t="s">
-        <v>30</v>
+        <v>130</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="B107">
-        <v>38.5</v>
+        <v>39.725000000000001</v>
       </c>
       <c r="C107">
-        <v>38.5</v>
+        <v>121.25</v>
       </c>
       <c r="D107">
-        <v>0.71</v>
+        <v>0.36499999999999999</v>
       </c>
       <c r="E107">
-        <v>0.71</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="F107">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G107" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="B108">
-        <v>47.3</v>
+        <v>25.8</v>
       </c>
       <c r="C108">
-        <v>47.3</v>
+        <v>84.95</v>
       </c>
       <c r="D108">
-        <v>0.9</v>
+        <v>0.35</v>
       </c>
       <c r="E108">
-        <v>0.9</v>
+        <v>0.43</v>
       </c>
       <c r="F108">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G108" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="B109">
-        <v>23.1</v>
+        <v>38.5</v>
       </c>
       <c r="C109">
-        <v>78.599999999999994</v>
+        <v>38.5</v>
       </c>
       <c r="D109">
-        <v>0.70499999999999996</v>
+        <v>0.71</v>
       </c>
       <c r="E109">
-        <v>0.84</v>
+        <v>0.71</v>
       </c>
       <c r="F109">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G109" t="s">
-        <v>10</v>
+        <v>138</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="B110">
-        <v>21.75</v>
+        <v>47.3</v>
       </c>
       <c r="C110">
-        <v>65.400000000000006</v>
+        <v>47.3</v>
       </c>
       <c r="D110">
-        <v>0.81499999999999995</v>
+        <v>0.9</v>
       </c>
       <c r="E110">
-        <v>0.995</v>
+        <v>0.9</v>
       </c>
       <c r="F110">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G110" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="B111">
-        <v>9.65</v>
+        <v>25.9</v>
       </c>
       <c r="C111">
-        <v>30.58</v>
+        <v>71.099999999999994</v>
       </c>
       <c r="D111">
-        <v>0.83499999999999996</v>
+        <v>0.71</v>
       </c>
       <c r="E111">
-        <v>0.94</v>
+        <v>0.84</v>
       </c>
       <c r="F111">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="G111" t="s">
-        <v>30</v>
+        <v>129</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="B112">
-        <v>121.4</v>
+        <v>19.675000000000001</v>
       </c>
       <c r="C112">
-        <v>150.19999999999999</v>
+        <v>67.099999999999994</v>
       </c>
       <c r="D112">
-        <v>0.44500000000000001</v>
+        <v>0.8125</v>
       </c>
       <c r="E112">
-        <v>0.73499999999999999</v>
+        <v>0.99</v>
       </c>
       <c r="F112">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G112" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="B113">
-        <v>1695</v>
+        <v>9</v>
       </c>
       <c r="C113">
-        <v>3264</v>
+        <v>29.274999999999999</v>
       </c>
       <c r="D113">
-        <v>0.74750000000000005</v>
+        <v>0.83</v>
       </c>
       <c r="E113">
-        <v>0.84250000000000003</v>
+        <v>0.94</v>
       </c>
       <c r="F113">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="G113" t="s">
         <v>86</v>
@@ -3874,186 +3876,232 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="B114">
-        <v>31.3</v>
+        <v>83.474999999999994</v>
       </c>
       <c r="C114">
-        <v>74.650000000000006</v>
+        <v>144.9</v>
       </c>
       <c r="D114">
-        <v>0.80500000000000005</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="E114">
-        <v>0.9</v>
+        <v>0.6875</v>
       </c>
       <c r="F114">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G114" t="s">
-        <v>21</v>
+        <v>140</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="B115">
-        <v>42.28</v>
+        <v>1694.8</v>
       </c>
       <c r="C115">
-        <v>67.03</v>
+        <v>3264.2</v>
       </c>
       <c r="D115">
-        <v>0.55500000000000005</v>
+        <v>0.74750000000000005</v>
       </c>
       <c r="E115">
-        <v>0.64500000000000002</v>
+        <v>0.84250000000000003</v>
       </c>
       <c r="F115">
         <v>2</v>
       </c>
       <c r="G115" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="B116">
-        <v>13.42</v>
+        <v>31.3</v>
       </c>
       <c r="C116">
-        <v>35.28</v>
+        <v>74.650000000000006</v>
       </c>
       <c r="D116">
-        <v>0.84499999999999997</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="E116">
-        <v>0.94750000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="F116">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="G116" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B117">
-        <v>23.25</v>
+        <v>42.274999999999999</v>
       </c>
       <c r="C117">
-        <v>89.6</v>
+        <v>67.025000000000006</v>
       </c>
       <c r="D117">
-        <v>0.73</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="E117">
-        <v>0.89500000000000002</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="F117">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="G117" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B118">
-        <v>39.17</v>
+        <v>13</v>
       </c>
       <c r="C118">
-        <v>104.2</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="D118">
-        <v>0.65</v>
+        <v>0.84</v>
       </c>
       <c r="E118">
-        <v>0.88</v>
+        <v>0.95</v>
       </c>
       <c r="F118">
-        <v>244</v>
+        <v>25</v>
       </c>
       <c r="G118" t="s">
-        <v>30</v>
+        <v>142</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B119">
-        <v>20.32</v>
+        <v>23.2</v>
       </c>
       <c r="C119">
-        <v>33.58</v>
+        <v>80</v>
       </c>
       <c r="D119">
-        <v>0.82</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="E119">
-        <v>0.88</v>
+        <v>0.89249999999999996</v>
       </c>
       <c r="F119">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="G119" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B120">
-        <v>12.05</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="C120">
-        <v>55.28</v>
+        <v>100.5</v>
       </c>
       <c r="D120">
-        <v>0.86250000000000004</v>
+        <v>0.66249999999999998</v>
       </c>
       <c r="E120">
-        <v>0.90749999999999997</v>
+        <v>0.88</v>
       </c>
       <c r="F120">
-        <v>10</v>
+        <v>274</v>
       </c>
       <c r="G120" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B121">
-        <v>33.119999999999997</v>
+        <v>20.324999999999999</v>
       </c>
       <c r="C121">
+        <v>33.575000000000003</v>
+      </c>
+      <c r="D121">
+        <v>0.82</v>
+      </c>
+      <c r="E121">
+        <v>0.88</v>
+      </c>
+      <c r="F121">
+        <v>2</v>
+      </c>
+      <c r="G121" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>125</v>
+      </c>
+      <c r="B122">
+        <v>12.4</v>
+      </c>
+      <c r="C122">
+        <v>55.45</v>
+      </c>
+      <c r="D122">
+        <v>0.86</v>
+      </c>
+      <c r="E122">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="F122">
+        <v>11</v>
+      </c>
+      <c r="G122" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>126</v>
+      </c>
+      <c r="B123">
+        <v>33.125</v>
+      </c>
+      <c r="C123">
         <v>48.9</v>
       </c>
-      <c r="D121">
+      <c r="D123">
         <v>0.67749999999999999</v>
       </c>
-      <c r="E121">
+      <c r="E123">
         <v>0.89500000000000002</v>
       </c>
-      <c r="F121">
+      <c r="F123">
         <v>10</v>
       </c>
-      <c r="G121" t="s">
-        <v>7</v>
+      <c r="G123" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>